<commit_message>
Have used only "Like to learn" for matching. New output format.
</commit_message>
<xml_diff>
--- a/project/figs/Matches_170430.xlsx
+++ b/project/figs/Matches_170430.xlsx
@@ -1,20 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1155,10 +1148,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1170,7 +1164,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
     </fill>
   </fills>
   <borders count="1">
@@ -1185,745 +1179,406 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A27" sqref="A1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="50.5" style="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="350">
+    <row r="2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="350">
+    <row r="3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="350">
+    <row r="4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="350">
+    <row r="5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="350">
+    <row r="6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="350">
+    <row r="7">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="350">
+    <row r="8">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="350">
+    <row r="9">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="350">
+    <row r="10">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="350">
+    <row r="11">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="350">
+    <row r="12">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="350">
+    <row r="13">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="350">
+    <row r="14">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="350">
+    <row r="15">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="350">
+    <row r="16">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="350">
+    <row r="17">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="350">
+    <row r="18">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="350">
+    <row r="19">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="350">
+    <row r="20">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="350">
+    <row r="21">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="350">
+    <row r="22">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="350">
+    <row r="23">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="350">
+    <row r="24">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="350">
+    <row r="25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="350">
+    <row r="26">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="350">
+    <row r="27">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="350">
+    <row r="28">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="350">
+    <row r="29">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="350">
+    <row r="30">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="364">
+    <row r="31">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="350">
+    <row r="32">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="350">
+    <row r="33">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="350">
+    <row r="34">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="350">
+    <row r="35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>